<commit_message>
NaN correction in Excel
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226" filterPrivacy="true"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Datos" sheetId="1" r:id="rId1"/>
+    <sheet name="datos" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,9 +397,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -453,7 +453,7 @@
         <v>USD CRC</v>
       </c>
       <c r="C3" t="str">
-        <v>549.36</v>
+        <v/>
       </c>
       <c r="D3" t="str">
         <v/>
@@ -465,7 +465,7 @@
         <v>EUR USD</v>
       </c>
       <c r="G3">
-        <v>1.06044</v>
+        <v>1.06652</v>
       </c>
     </row>
     <row r="4">
@@ -475,8 +475,8 @@
       <c r="B4" t="str">
         <v>USD UYU</v>
       </c>
-      <c r="C4">
-        <v>39.496</v>
+      <c r="C4" t="str">
+        <v/>
       </c>
       <c r="D4" t="str">
         <v/>
@@ -488,7 +488,7 @@
         <v>EUR COP</v>
       </c>
       <c r="G4">
-        <v>5136.61</v>
+        <v>5163.49</v>
       </c>
     </row>
     <row r="5">
@@ -498,8 +498,8 @@
       <c r="B5" t="str">
         <v>USD COP</v>
       </c>
-      <c r="C5">
-        <v>0</v>
+      <c r="C5" t="str">
+        <v/>
       </c>
       <c r="D5" t="str">
         <v/>
@@ -511,7 +511,7 @@
         <v>CNY USD</v>
       </c>
       <c r="G5">
-        <v>0.1449</v>
+        <v>0.14518</v>
       </c>
     </row>
     <row r="6">
@@ -521,8 +521,8 @@
       <c r="B6" t="str">
         <v>USD PEN</v>
       </c>
-      <c r="C6">
-        <v>3.801</v>
+      <c r="C6" t="str">
+        <v/>
       </c>
       <c r="D6" t="str">
         <v/>
@@ -534,7 +534,7 @@
         <v>JPY USD</v>
       </c>
       <c r="G6">
-        <v>0.00752</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -544,8 +544,8 @@
       <c r="B7" t="str">
         <v>EUR PEN</v>
       </c>
-      <c r="C7">
-        <v>4.12</v>
+      <c r="C7" t="str">
+        <v/>
       </c>
       <c r="D7" t="str">
         <v/>
@@ -556,8 +556,8 @@
       <c r="F7" t="str">
         <v>CNY COP</v>
       </c>
-      <c r="G7">
-        <v>701.872</v>
+      <c r="G7" t="str">
+        <v/>
       </c>
     </row>
     <row r="8">
@@ -567,8 +567,8 @@
       <c r="B8" t="str">
         <v>USD CLP</v>
       </c>
-      <c r="C8">
-        <v>824.65</v>
+      <c r="C8" t="str">
+        <v/>
       </c>
       <c r="D8" t="str">
         <v/>
@@ -579,8 +579,8 @@
       <c r="F8" t="str">
         <v>JPY COP</v>
       </c>
-      <c r="G8">
-        <v>36.4138</v>
+      <c r="G8" t="str">
+        <v/>
       </c>
     </row>
     <row r="9">
@@ -590,8 +590,8 @@
       <c r="B9" t="str">
         <v>EUR CLP</v>
       </c>
-      <c r="C9">
-        <v>874.87</v>
+      <c r="C9" t="str">
+        <v/>
       </c>
       <c r="D9" t="str">
         <v/>
@@ -602,8 +602,8 @@
       <c r="F9" t="str">
         <v>BRL USD</v>
       </c>
-      <c r="G9">
-        <v>0.18952</v>
+      <c r="G9" t="str">
+        <v/>
       </c>
     </row>
     <row r="10">
@@ -613,8 +613,8 @@
       <c r="B10" t="str">
         <v>USD GTQ</v>
       </c>
-      <c r="C10">
-        <v>0</v>
+      <c r="C10" t="str">
+        <v/>
       </c>
       <c r="D10" t="str">
         <v/>
@@ -625,8 +625,8 @@
       <c r="F10" t="str">
         <v>KRW USD</v>
       </c>
-      <c r="G10">
-        <v>0.00076</v>
+      <c r="G10" t="str">
+        <v/>
       </c>
     </row>
     <row r="11">
@@ -636,6 +636,9 @@
       <c r="B11" t="str">
         <v>USD HNL</v>
       </c>
+      <c r="C11" t="str">
+        <v/>
+      </c>
       <c r="D11" t="str">
         <v/>
       </c>
@@ -645,196 +648,13 @@
       <c r="F11" t="str">
         <v>USD CLP</v>
       </c>
-      <c r="G11">
-        <v>823.124</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v/>
-      </c>
-      <c r="B12" t="str">
-        <v/>
-      </c>
-      <c r="C12" t="str">
-        <v/>
-      </c>
-      <c r="D12" t="str">
-        <v/>
-      </c>
-      <c r="E12" t="str">
-        <v/>
-      </c>
-      <c r="F12" t="str">
-        <v>EUR CLP</v>
-      </c>
-      <c r="G12">
-        <v>873.012</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v/>
-      </c>
-      <c r="B13" t="str">
-        <v/>
-      </c>
-      <c r="C13" t="str">
-        <v/>
-      </c>
-      <c r="D13" t="str">
-        <v/>
-      </c>
-      <c r="E13" t="str">
-        <v/>
-      </c>
-      <c r="F13" t="str">
-        <v>BRL HNL</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v/>
-      </c>
-      <c r="B14" t="str">
-        <v/>
-      </c>
-      <c r="C14" t="str">
-        <v/>
-      </c>
-      <c r="D14" t="str">
-        <v/>
-      </c>
-      <c r="E14" t="str">
-        <v/>
-      </c>
-      <c r="F14" t="str">
-        <v>CNY HNL</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v/>
-      </c>
-      <c r="B15" t="str">
-        <v/>
-      </c>
-      <c r="C15" t="str">
-        <v/>
-      </c>
-      <c r="D15" t="str">
-        <v/>
-      </c>
-      <c r="E15" t="str">
-        <v/>
-      </c>
-      <c r="F15" t="str">
-        <v>EUR HNL</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="str">
-        <v/>
-      </c>
-      <c r="B16" t="str">
-        <v/>
-      </c>
-      <c r="C16" t="str">
-        <v/>
-      </c>
-      <c r="D16" t="str">
-        <v/>
-      </c>
-      <c r="E16" t="str">
-        <v/>
-      </c>
-      <c r="F16" t="str">
-        <v>GBP HNL</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="str">
-        <v/>
-      </c>
-      <c r="B17" t="str">
-        <v/>
-      </c>
-      <c r="C17" t="str">
-        <v/>
-      </c>
-      <c r="D17" t="str">
-        <v/>
-      </c>
-      <c r="E17" t="str">
-        <v/>
-      </c>
-      <c r="F17" t="str">
-        <v>JPY HNL</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="str">
-        <v/>
-      </c>
-      <c r="B18" t="str">
-        <v/>
-      </c>
-      <c r="C18" t="str">
-        <v/>
-      </c>
-      <c r="D18" t="str">
-        <v/>
-      </c>
-      <c r="E18" t="str">
-        <v/>
-      </c>
-      <c r="F18" t="str">
-        <v>MXN HNL</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="str">
-        <v/>
-      </c>
-      <c r="B19" t="str">
-        <v/>
-      </c>
-      <c r="C19" t="str">
-        <v/>
-      </c>
-      <c r="D19" t="str">
-        <v/>
-      </c>
-      <c r="E19" t="str">
-        <v/>
-      </c>
-      <c r="F19" t="str">
-        <v>HKD USD</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="str">
-        <v/>
-      </c>
-      <c r="B20" t="str">
-        <v/>
-      </c>
-      <c r="C20" t="str">
-        <v/>
-      </c>
-      <c r="D20" t="str">
-        <v/>
-      </c>
-      <c r="E20" t="str">
-        <v/>
-      </c>
-      <c r="F20" t="str">
-        <v>HKD HNL</v>
+      <c r="G11" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G20"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Correctly Nan Version 1.1
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -465,7 +465,7 @@
         <v>EUR USD</v>
       </c>
       <c r="G3">
-        <v>1.06652</v>
+        <v>1.07184</v>
       </c>
     </row>
     <row r="4">
@@ -488,7 +488,7 @@
         <v>EUR COP</v>
       </c>
       <c r="G4">
-        <v>5163.49</v>
+        <v>5173.63</v>
       </c>
     </row>
     <row r="5">
@@ -511,7 +511,7 @@
         <v>CNY USD</v>
       </c>
       <c r="G5">
-        <v>0.14518</v>
+        <v>0.14522</v>
       </c>
     </row>
     <row r="6">
@@ -534,7 +534,7 @@
         <v>JPY USD</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>0.0076</v>
       </c>
     </row>
     <row r="7">

</xml_diff>